<commit_message>
update spreadsheet according to input order
</commit_message>
<xml_diff>
--- a/units.xlsx
+++ b/units.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t xml:space="preserve">Unit Class</t>
   </si>
@@ -43,6 +43,15 @@
     <t xml:space="preserve">tank</t>
   </si>
   <si>
+    <t xml:space="preserve">AFV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FA</t>
+  </si>
+  <si>
     <t xml:space="preserve">air</t>
   </si>
   <si>
@@ -50,9 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">bomber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AFV</t>
   </si>
   <si>
     <t xml:space="preserve">naval</t>
@@ -85,6 +91,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -106,6 +113,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,12 +158,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -176,13 +188,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -199,142 +211,170 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="2" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="2" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="C4" s="0" t="n">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="C5" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D5" s="0" t="n">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="0" t="n">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D9" s="2" t="n">
         <v>60</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="0" t="n">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D10" s="2" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="0" t="n">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2" t="n">
         <v>45</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D11" s="2" t="n">
         <v>45</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="0" t="n">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D12" s="2" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="0" t="n">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D13" s="2" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add personnel and casualty factors to units
</commit_message>
<xml_diff>
--- a/units.xlsx
+++ b/units.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t xml:space="preserve">Unit Class</t>
   </si>
@@ -32,6 +32,15 @@
   </si>
   <si>
     <t xml:space="preserve">Attack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casualty Factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conscript Casualty Factor</t>
   </si>
   <si>
     <t xml:space="preserve">land</t>
@@ -188,13 +197,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -209,13 +218,22 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>2</v>
@@ -223,13 +241,22 @@
       <c r="D2" s="2" t="n">
         <v>5</v>
       </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>15</v>
@@ -237,13 +264,22 @@
       <c r="D3" s="2" t="n">
         <v>15</v>
       </c>
+      <c r="E3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>10</v>
@@ -251,13 +287,22 @@
       <c r="D4" s="2" t="n">
         <v>8</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>6</v>
@@ -265,13 +310,22 @@
       <c r="D5" s="2" t="n">
         <v>15</v>
       </c>
+      <c r="E5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>6</v>
@@ -279,13 +333,22 @@
       <c r="D6" s="2" t="n">
         <v>25</v>
       </c>
+      <c r="E6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>8</v>
@@ -293,13 +356,22 @@
       <c r="D7" s="2" t="n">
         <v>12</v>
       </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>10</v>
@@ -307,13 +379,22 @@
       <c r="D8" s="2" t="n">
         <v>20</v>
       </c>
+      <c r="E8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>60</v>
@@ -321,13 +402,22 @@
       <c r="D9" s="2" t="n">
         <v>60</v>
       </c>
+      <c r="E9" s="0" t="n">
+        <v>850</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>30</v>
@@ -335,13 +425,22 @@
       <c r="D10" s="2" t="n">
         <v>40</v>
       </c>
+      <c r="E10" s="0" t="n">
+        <v>450</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>45</v>
@@ -349,13 +448,22 @@
       <c r="D11" s="2" t="n">
         <v>45</v>
       </c>
+      <c r="E11" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>30</v>
@@ -363,19 +471,37 @@
       <c r="D12" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="E12" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>30</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>